<commit_message>
Dynamically mapping table type to model type (Factory method)
</commit_message>
<xml_diff>
--- a/src/main/resources/Paysheet.xlsx
+++ b/src/main/resources/Paysheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhammika Mahendra\Documents\Code Test\Java\SpringMVC\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D5540-405C-474B-9DD0-D5A77A1BEE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C7165C-5671-4F1F-BDB2-BF4D0C6067C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1BDCFAD9-094C-48DB-BED5-9F51F545E0C9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>PAYMENT_ID</t>
   </si>
@@ -38,18 +38,6 @@
   </si>
   <si>
     <t>CREDIT_CARD</t>
-  </si>
-  <si>
-    <t>COMPLETED</t>
-  </si>
-  <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>DEBIT_CARD</t>
   </si>
   <si>
     <t>REFUNDED</t>
@@ -536,9 +524,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -917,7 +906,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,8 +937,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>125.5</v>
+      <c r="B2" s="2">
+        <v>5000</v>
       </c>
       <c r="C2" s="1">
         <v>45347.604166666664</v>
@@ -965,48 +954,48 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>89.99</v>
+      <c r="B3" s="2">
+        <v>5000</v>
       </c>
       <c r="C3" s="1">
         <v>45346.385416666664</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>200</v>
+      <c r="B4" s="2">
+        <v>5000</v>
       </c>
       <c r="C4" s="1">
         <v>45345.78125</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>49.75</v>
+      <c r="B5" s="2">
+        <v>5000</v>
       </c>
       <c r="C5" s="1">
         <v>45344.506944444445</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -1016,17 +1005,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>300.25</v>
+      <c r="B6" s="2">
+        <v>5000</v>
       </c>
       <c r="C6" s="1">
         <v>45343.704861111109</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>